<commit_message>
New experiments results - up to 4000 seconds
</commit_message>
<xml_diff>
--- a/extensions/dVMP-JournalExtension-July2016/doc-Experiments/ResultsAbstracts.xlsx
+++ b/extensions/dVMP-JournalExtension-July2016/doc-Experiments/ResultsAbstracts.xlsx
@@ -745,54 +745,6 @@
                 <c:pt idx="44">
                   <c:v>4053.532168361</c:v>
                 </c:pt>
-                <c:pt idx="45">
-                  <c:v>4136.68382201</c:v>
-                </c:pt>
-                <c:pt idx="46">
-                  <c:v>4220.810813569</c:v>
-                </c:pt>
-                <c:pt idx="47">
-                  <c:v>4303.945301235</c:v>
-                </c:pt>
-                <c:pt idx="48">
-                  <c:v>4385.917480131</c:v>
-                </c:pt>
-                <c:pt idx="49">
-                  <c:v>4469.108390695</c:v>
-                </c:pt>
-                <c:pt idx="50">
-                  <c:v>4552.900793191</c:v>
-                </c:pt>
-                <c:pt idx="51">
-                  <c:v>4637.644676554</c:v>
-                </c:pt>
-                <c:pt idx="52">
-                  <c:v>4721.633628043</c:v>
-                </c:pt>
-                <c:pt idx="53">
-                  <c:v>4804.771710631</c:v>
-                </c:pt>
-                <c:pt idx="54">
-                  <c:v>4887.537935356</c:v>
-                </c:pt>
-                <c:pt idx="55">
-                  <c:v>4972.525393161</c:v>
-                </c:pt>
-                <c:pt idx="56">
-                  <c:v>5056.461062461</c:v>
-                </c:pt>
-                <c:pt idx="57">
-                  <c:v>5139.085390246</c:v>
-                </c:pt>
-                <c:pt idx="58">
-                  <c:v>5222.466200951</c:v>
-                </c:pt>
-                <c:pt idx="59">
-                  <c:v>5306.495611442</c:v>
-                </c:pt>
-                <c:pt idx="60">
-                  <c:v>5389.470699607</c:v>
-                </c:pt>
               </c:numCache>
             </c:numRef>
           </c:xVal>
@@ -936,54 +888,6 @@
                 </c:pt>
                 <c:pt idx="44">
                   <c:v>-8.95822896509299E7</c:v>
-                </c:pt>
-                <c:pt idx="45">
-                  <c:v>-8.95677263277831E7</c:v>
-                </c:pt>
-                <c:pt idx="46">
-                  <c:v>-8.95289758621852E7</c:v>
-                </c:pt>
-                <c:pt idx="47">
-                  <c:v>-8.94996152917373E7</c:v>
-                </c:pt>
-                <c:pt idx="48">
-                  <c:v>-8.94737786536254E7</c:v>
-                </c:pt>
-                <c:pt idx="49">
-                  <c:v>-8.946526199169E7</c:v>
-                </c:pt>
-                <c:pt idx="50">
-                  <c:v>-8.94449351056094E7</c:v>
-                </c:pt>
-                <c:pt idx="51">
-                  <c:v>-8.94132649372153E7</c:v>
-                </c:pt>
-                <c:pt idx="52">
-                  <c:v>-8.93841720435364E7</c:v>
-                </c:pt>
-                <c:pt idx="53">
-                  <c:v>-8.93732823425349E7</c:v>
-                </c:pt>
-                <c:pt idx="54">
-                  <c:v>-8.93499072712077E7</c:v>
-                </c:pt>
-                <c:pt idx="55">
-                  <c:v>-8.93260987166988E7</c:v>
-                </c:pt>
-                <c:pt idx="56">
-                  <c:v>-8.93091143329133E7</c:v>
-                </c:pt>
-                <c:pt idx="57">
-                  <c:v>-8.92889078483163E7</c:v>
-                </c:pt>
-                <c:pt idx="58">
-                  <c:v>-8.92817633628116E7</c:v>
-                </c:pt>
-                <c:pt idx="59">
-                  <c:v>-8.92649327454865E7</c:v>
-                </c:pt>
-                <c:pt idx="60">
-                  <c:v>-8.92532370876559E7</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1134,54 +1038,6 @@
                 <c:pt idx="44">
                   <c:v>4038.678758877</c:v>
                 </c:pt>
-                <c:pt idx="45">
-                  <c:v>4121.195089152</c:v>
-                </c:pt>
-                <c:pt idx="46">
-                  <c:v>4202.812153689</c:v>
-                </c:pt>
-                <c:pt idx="47">
-                  <c:v>4285.801659929</c:v>
-                </c:pt>
-                <c:pt idx="48">
-                  <c:v>4367.621974569</c:v>
-                </c:pt>
-                <c:pt idx="49">
-                  <c:v>4450.106113018</c:v>
-                </c:pt>
-                <c:pt idx="50">
-                  <c:v>4532.903472765001</c:v>
-                </c:pt>
-                <c:pt idx="51">
-                  <c:v>4613.192754835</c:v>
-                </c:pt>
-                <c:pt idx="52">
-                  <c:v>4694.85495072</c:v>
-                </c:pt>
-                <c:pt idx="53">
-                  <c:v>4777.777363083001</c:v>
-                </c:pt>
-                <c:pt idx="54">
-                  <c:v>4859.149184956</c:v>
-                </c:pt>
-                <c:pt idx="55">
-                  <c:v>4942.756370663</c:v>
-                </c:pt>
-                <c:pt idx="56">
-                  <c:v>5025.458875982</c:v>
-                </c:pt>
-                <c:pt idx="57">
-                  <c:v>5107.913122411</c:v>
-                </c:pt>
-                <c:pt idx="58">
-                  <c:v>5190.489975849</c:v>
-                </c:pt>
-                <c:pt idx="59">
-                  <c:v>5272.031607307001</c:v>
-                </c:pt>
-                <c:pt idx="60">
-                  <c:v>5355.137332181001</c:v>
-                </c:pt>
               </c:numCache>
             </c:numRef>
           </c:xVal>
@@ -1325,54 +1181,6 @@
                 </c:pt>
                 <c:pt idx="44">
                   <c:v>-9.05607589203108E7</c:v>
-                </c:pt>
-                <c:pt idx="45">
-                  <c:v>-9.05290877474483E7</c:v>
-                </c:pt>
-                <c:pt idx="46">
-                  <c:v>-9.04843059717212E7</c:v>
-                </c:pt>
-                <c:pt idx="47">
-                  <c:v>-9.0469576553931E7</c:v>
-                </c:pt>
-                <c:pt idx="48">
-                  <c:v>-9.04503715051305E7</c:v>
-                </c:pt>
-                <c:pt idx="49">
-                  <c:v>-9.04026012007134E7</c:v>
-                </c:pt>
-                <c:pt idx="50">
-                  <c:v>-9.03371859232132E7</c:v>
-                </c:pt>
-                <c:pt idx="51">
-                  <c:v>-9.03024656008902E7</c:v>
-                </c:pt>
-                <c:pt idx="52">
-                  <c:v>-9.02911401405968E7</c:v>
-                </c:pt>
-                <c:pt idx="53">
-                  <c:v>-9.02625461394379E7</c:v>
-                </c:pt>
-                <c:pt idx="54">
-                  <c:v>-9.02019808422764E7</c:v>
-                </c:pt>
-                <c:pt idx="55">
-                  <c:v>-9.0161545367942E7</c:v>
-                </c:pt>
-                <c:pt idx="56">
-                  <c:v>-9.01432078326398E7</c:v>
-                </c:pt>
-                <c:pt idx="57">
-                  <c:v>-9.01176342312372E7</c:v>
-                </c:pt>
-                <c:pt idx="58">
-                  <c:v>-9.00958097919118E7</c:v>
-                </c:pt>
-                <c:pt idx="59">
-                  <c:v>-9.00614172418697E7</c:v>
-                </c:pt>
-                <c:pt idx="60">
-                  <c:v>-9.00307301552911E7</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1529,57 +1337,6 @@
                 <c:pt idx="46">
                   <c:v>4074.433624215</c:v>
                 </c:pt>
-                <c:pt idx="47">
-                  <c:v>4153.512226451</c:v>
-                </c:pt>
-                <c:pt idx="48">
-                  <c:v>4232.537610928001</c:v>
-                </c:pt>
-                <c:pt idx="49">
-                  <c:v>4313.807475889</c:v>
-                </c:pt>
-                <c:pt idx="50">
-                  <c:v>4393.311612729</c:v>
-                </c:pt>
-                <c:pt idx="51">
-                  <c:v>4472.889232356</c:v>
-                </c:pt>
-                <c:pt idx="52">
-                  <c:v>4553.896471398</c:v>
-                </c:pt>
-                <c:pt idx="53">
-                  <c:v>4633.696171357</c:v>
-                </c:pt>
-                <c:pt idx="54">
-                  <c:v>4715.010542598</c:v>
-                </c:pt>
-                <c:pt idx="55">
-                  <c:v>4796.191576134</c:v>
-                </c:pt>
-                <c:pt idx="56">
-                  <c:v>4876.577577281</c:v>
-                </c:pt>
-                <c:pt idx="57">
-                  <c:v>4956.414402669</c:v>
-                </c:pt>
-                <c:pt idx="58">
-                  <c:v>5037.121045119</c:v>
-                </c:pt>
-                <c:pt idx="59">
-                  <c:v>5117.488087583</c:v>
-                </c:pt>
-                <c:pt idx="60">
-                  <c:v>5197.363002618</c:v>
-                </c:pt>
-                <c:pt idx="61">
-                  <c:v>5278.218975913001</c:v>
-                </c:pt>
-                <c:pt idx="62">
-                  <c:v>5359.543157244</c:v>
-                </c:pt>
-                <c:pt idx="63">
-                  <c:v>5440.367380745</c:v>
-                </c:pt>
               </c:numCache>
             </c:numRef>
           </c:xVal>
@@ -1729,57 +1486,6 @@
                 </c:pt>
                 <c:pt idx="46">
                   <c:v>-9.01043187035452E7</c:v>
-                </c:pt>
-                <c:pt idx="47">
-                  <c:v>-9.00805952953502E7</c:v>
-                </c:pt>
-                <c:pt idx="48">
-                  <c:v>-9.00652232926578E7</c:v>
-                </c:pt>
-                <c:pt idx="49">
-                  <c:v>-9.00339112772436E7</c:v>
-                </c:pt>
-                <c:pt idx="50">
-                  <c:v>-9.00120520347148E7</c:v>
-                </c:pt>
-                <c:pt idx="51">
-                  <c:v>-8.99875868309226E7</c:v>
-                </c:pt>
-                <c:pt idx="52">
-                  <c:v>-8.99744796850311E7</c:v>
-                </c:pt>
-                <c:pt idx="53">
-                  <c:v>-8.99653843315779E7</c:v>
-                </c:pt>
-                <c:pt idx="54">
-                  <c:v>-8.99492219351112E7</c:v>
-                </c:pt>
-                <c:pt idx="55">
-                  <c:v>-8.99308254663567E7</c:v>
-                </c:pt>
-                <c:pt idx="56">
-                  <c:v>-8.99165141648739E7</c:v>
-                </c:pt>
-                <c:pt idx="57">
-                  <c:v>-8.99036263220979E7</c:v>
-                </c:pt>
-                <c:pt idx="58">
-                  <c:v>-8.98930313704487E7</c:v>
-                </c:pt>
-                <c:pt idx="59">
-                  <c:v>-8.98828996396127E7</c:v>
-                </c:pt>
-                <c:pt idx="60">
-                  <c:v>-8.98575897360412E7</c:v>
-                </c:pt>
-                <c:pt idx="61">
-                  <c:v>-8.9853080026942E7</c:v>
-                </c:pt>
-                <c:pt idx="62">
-                  <c:v>-8.98474393011135E7</c:v>
-                </c:pt>
-                <c:pt idx="63">
-                  <c:v>-8.98232523975237E7</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -12157,8 +11863,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:O98"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="D1" workbookViewId="0">
-      <selection activeCell="J3" sqref="J3:L65"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B46" sqref="A33:B46"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -12277,21 +11983,21 @@
         <f>$C$2+M3</f>
         <v>480.23369023100003</v>
       </c>
-      <c r="D3" s="1">
+      <c r="D3" s="5">
         <v>-352598756.43099499</v>
       </c>
       <c r="E3" s="4">
         <f>$C$2+N3</f>
         <v>481.82593134700005</v>
       </c>
-      <c r="F3" s="1">
+      <c r="F3" s="5">
         <v>-362667710.25365502</v>
       </c>
       <c r="G3" s="4">
         <f>$C$2+O3</f>
         <v>482.181607348</v>
       </c>
-      <c r="H3" s="1">
+      <c r="H3" s="5">
         <v>-364384002.06646901</v>
       </c>
       <c r="I3" s="4">
@@ -12310,7 +12016,7 @@
         <f>$D$2/H3</f>
         <v>0.32782528098837821</v>
       </c>
-      <c r="M3" s="1">
+      <c r="M3">
         <v>9.4043991299999998</v>
       </c>
       <c r="N3">
@@ -12331,21 +12037,21 @@
         <f t="shared" ref="C4:C62" si="1">$C$2+M4</f>
         <v>563.67819973500002</v>
       </c>
-      <c r="D4" s="1">
+      <c r="D4" s="5">
         <v>-131189144.72922701</v>
       </c>
       <c r="E4" s="4">
         <f t="shared" ref="E4:E62" si="2">$C$2+N4</f>
         <v>564.879195665</v>
       </c>
-      <c r="F4" s="1">
+      <c r="F4" s="5">
         <v>-134689112.41765699</v>
       </c>
       <c r="G4" s="4">
         <f t="shared" ref="G4:G65" si="3">$C$2+O4</f>
         <v>566.56038626700001</v>
       </c>
-      <c r="H4" s="1">
+      <c r="H4" s="5">
         <v>-133012512.44134501</v>
       </c>
       <c r="I4" s="4">
@@ -12364,7 +12070,7 @@
         <f t="shared" ref="L4:L65" si="6">$D$2/H4</f>
         <v>0.89806805143828983</v>
       </c>
-      <c r="M4" s="1">
+      <c r="M4">
         <v>92.848908633999997</v>
       </c>
       <c r="N4">
@@ -12385,21 +12091,21 @@
         <f t="shared" si="1"/>
         <v>644.88397852900005</v>
       </c>
-      <c r="D5" s="1">
+      <c r="D5" s="5">
         <v>-113395552.590992</v>
       </c>
       <c r="E5" s="4">
         <f t="shared" si="2"/>
         <v>645.68671370600009</v>
       </c>
-      <c r="F5" s="1">
+      <c r="F5" s="5">
         <v>-113933745.031427</v>
       </c>
       <c r="G5" s="4">
         <f t="shared" si="3"/>
         <v>646.90465366300009</v>
       </c>
-      <c r="H5" s="1">
+      <c r="H5" s="5">
         <v>-113655608.355121</v>
       </c>
       <c r="I5" s="4">
@@ -12418,7 +12124,7 @@
         <f t="shared" si="6"/>
         <v>1.0510197393152023</v>
       </c>
-      <c r="M5" s="1">
+      <c r="M5">
         <v>174.05468742799999</v>
       </c>
       <c r="N5">
@@ -12439,21 +12145,21 @@
         <f t="shared" si="1"/>
         <v>725.60157292899999</v>
       </c>
-      <c r="D6" s="1">
+      <c r="D6" s="5">
         <v>-105847414.599153</v>
       </c>
       <c r="E6" s="4">
         <f t="shared" si="2"/>
         <v>728.40469184600011</v>
       </c>
-      <c r="F6" s="1">
+      <c r="F6" s="5">
         <v>-106252597.942702</v>
       </c>
       <c r="G6" s="4">
         <f t="shared" si="3"/>
         <v>725.53114435999998</v>
       </c>
-      <c r="H6" s="1">
+      <c r="H6" s="5">
         <v>-106743776.697705</v>
       </c>
       <c r="I6" s="4">
@@ -12472,7 +12178,7 @@
         <f t="shared" si="6"/>
         <v>1.1190749621254339</v>
       </c>
-      <c r="M6" s="1">
+      <c r="M6">
         <v>254.77228182799999</v>
       </c>
       <c r="N6">
@@ -12493,21 +12199,21 @@
         <f t="shared" si="1"/>
         <v>806.6129168330001</v>
       </c>
-      <c r="D7" s="1">
+      <c r="D7" s="5">
         <v>-101809745.474315</v>
       </c>
       <c r="E7" s="4">
         <f t="shared" si="2"/>
         <v>810.93050069000003</v>
       </c>
-      <c r="F7" s="1">
+      <c r="F7" s="5">
         <v>-102676044.564674</v>
       </c>
       <c r="G7" s="4">
         <f t="shared" si="3"/>
         <v>804.81916009099996</v>
       </c>
-      <c r="H7" s="1">
+      <c r="H7" s="5">
         <v>-102427580.177799</v>
       </c>
       <c r="I7" s="4">
@@ -12526,7 +12232,7 @@
         <f t="shared" si="6"/>
         <v>1.1662316698076356</v>
       </c>
-      <c r="M7" s="1">
+      <c r="M7">
         <v>335.78362573200002</v>
       </c>
       <c r="N7">
@@ -12547,21 +12253,21 @@
         <f t="shared" si="1"/>
         <v>888.73997338899994</v>
       </c>
-      <c r="D8" s="1">
+      <c r="D8" s="5">
         <v>-99155527.235931396</v>
       </c>
       <c r="E8" s="4">
         <f t="shared" si="2"/>
         <v>891.45526840900004</v>
       </c>
-      <c r="F8" s="1">
+      <c r="F8" s="5">
         <v>-100719014.228874</v>
       </c>
       <c r="G8" s="4">
         <f t="shared" si="3"/>
         <v>884.36341968900001</v>
       </c>
-      <c r="H8" s="1">
+      <c r="H8" s="5">
         <v>-99766235.346898302</v>
       </c>
       <c r="I8" s="4">
@@ -12580,7 +12286,7 @@
         <f t="shared" si="6"/>
         <v>1.1973418406513401</v>
       </c>
-      <c r="M8" s="1">
+      <c r="M8">
         <v>417.91068228799998</v>
       </c>
       <c r="N8">
@@ -12601,21 +12307,21 @@
         <f t="shared" si="1"/>
         <v>969.88316035499997</v>
       </c>
-      <c r="D9" s="1">
+      <c r="D9" s="5">
         <v>-97285578.531598896</v>
       </c>
       <c r="E9" s="4">
         <f t="shared" si="2"/>
         <v>972.78000647299996</v>
       </c>
-      <c r="F9" s="1">
+      <c r="F9" s="5">
         <v>-99187327.190032497</v>
       </c>
       <c r="G9" s="4">
         <f t="shared" si="3"/>
         <v>963.73600271300006</v>
       </c>
-      <c r="H9" s="1">
+      <c r="H9" s="5">
         <v>-97891936.682404399</v>
       </c>
       <c r="I9" s="4">
@@ -12634,7 +12340,7 @@
         <f t="shared" si="6"/>
         <v>1.2202668770632394</v>
       </c>
-      <c r="M9" s="1">
+      <c r="M9">
         <v>499.05386925400001</v>
       </c>
       <c r="N9">
@@ -12655,21 +12361,21 @@
         <f t="shared" si="1"/>
         <v>1052.669295485</v>
       </c>
-      <c r="D10" s="1">
+      <c r="D10" s="5">
         <v>-95979907.620125994</v>
       </c>
       <c r="E10" s="4">
         <f t="shared" si="2"/>
         <v>1054.4945590780001</v>
       </c>
-      <c r="F10" s="1">
+      <c r="F10" s="5">
         <v>-97947093.476735502</v>
       </c>
       <c r="G10" s="4">
         <f t="shared" si="3"/>
         <v>1043.2940154160001</v>
       </c>
-      <c r="H10" s="1">
+      <c r="H10" s="5">
         <v>-96619555.972393095</v>
       </c>
       <c r="I10" s="4">
@@ -12688,7 +12394,7 @@
         <f t="shared" si="6"/>
         <v>1.2363365434968612</v>
       </c>
-      <c r="M10" s="1">
+      <c r="M10">
         <v>581.84000438400005</v>
       </c>
       <c r="N10">
@@ -12709,21 +12415,21 @@
         <f t="shared" si="1"/>
         <v>1133.9341321209999</v>
       </c>
-      <c r="D11" s="1">
+      <c r="D11" s="5">
         <v>-95199969.516283303</v>
       </c>
       <c r="E11" s="4">
         <f t="shared" si="2"/>
         <v>1136.0026622739999</v>
       </c>
-      <c r="F11" s="1">
+      <c r="F11" s="5">
         <v>-97014793.399956197</v>
       </c>
       <c r="G11" s="4">
         <f t="shared" si="3"/>
         <v>1122.1432854940001</v>
       </c>
-      <c r="H11" s="1">
+      <c r="H11" s="5">
         <v>-95679487.485807195</v>
       </c>
       <c r="I11" s="4">
@@ -12742,7 +12448,7 @@
         <f t="shared" si="6"/>
         <v>1.2484837764503023</v>
       </c>
-      <c r="M11" s="1">
+      <c r="M11">
         <v>663.10484101999998</v>
       </c>
       <c r="N11">
@@ -12763,21 +12469,21 @@
         <f t="shared" si="1"/>
         <v>1216.9907128279999</v>
       </c>
-      <c r="D12" s="1">
+      <c r="D12" s="5">
         <v>-94468134.0740913</v>
       </c>
       <c r="E12" s="4">
         <f t="shared" si="2"/>
         <v>1218.5334985950001</v>
       </c>
-      <c r="F12" s="1">
+      <c r="F12" s="5">
         <v>-96173769.264624</v>
       </c>
       <c r="G12" s="4">
         <f t="shared" si="3"/>
         <v>1202.3039986040001</v>
       </c>
-      <c r="H12" s="1">
+      <c r="H12" s="5">
         <v>-94937224.042777494</v>
       </c>
       <c r="I12" s="4">
@@ -12796,7 +12502,7 @@
         <f t="shared" si="6"/>
         <v>1.2582450042070477</v>
       </c>
-      <c r="M12" s="1">
+      <c r="M12">
         <v>746.16142172699995</v>
       </c>
       <c r="N12">
@@ -12817,21 +12523,21 @@
         <f t="shared" si="1"/>
         <v>1301.6213964860001</v>
       </c>
-      <c r="D13" s="1">
+      <c r="D13" s="5">
         <v>-93855386.561150104</v>
       </c>
       <c r="E13" s="4">
         <f t="shared" si="2"/>
         <v>1300.961099786</v>
       </c>
-      <c r="F13" s="1">
+      <c r="F13" s="5">
         <v>-95622394.363075197</v>
       </c>
       <c r="G13" s="4">
         <f t="shared" si="3"/>
         <v>1283.1857853430001</v>
       </c>
-      <c r="H13" s="1">
+      <c r="H13" s="5">
         <v>-94299399.217476398</v>
       </c>
       <c r="I13" s="4">
@@ -12850,7 +12556,7 @@
         <f t="shared" si="6"/>
         <v>1.2667555557763477</v>
       </c>
-      <c r="M13" s="1">
+      <c r="M13">
         <v>830.79210538500001</v>
       </c>
       <c r="N13">
@@ -12871,21 +12577,21 @@
         <f t="shared" si="1"/>
         <v>1384.096790991</v>
       </c>
-      <c r="D14" s="1">
+      <c r="D14" s="5">
         <v>-93361916.529450998</v>
       </c>
       <c r="E14" s="4">
         <f t="shared" si="2"/>
         <v>1383.3750627720001</v>
       </c>
-      <c r="F14" s="1">
+      <c r="F14" s="5">
         <v>-95173348.458831102</v>
       </c>
       <c r="G14" s="4">
         <f t="shared" si="3"/>
         <v>1361.9045659810001</v>
       </c>
-      <c r="H14" s="1">
+      <c r="H14" s="5">
         <v>-93677686.1953789</v>
       </c>
       <c r="I14" s="4">
@@ -12904,7 +12610,7 @@
         <f t="shared" si="6"/>
         <v>1.275162663774275</v>
       </c>
-      <c r="M14" s="1">
+      <c r="M14">
         <v>913.26749988999995</v>
       </c>
       <c r="N14">
@@ -12925,21 +12631,21 @@
         <f t="shared" si="1"/>
         <v>1466.854596979</v>
       </c>
-      <c r="D15" s="1">
+      <c r="D15" s="5">
         <v>-92931878.726144999</v>
       </c>
       <c r="E15" s="4">
         <f t="shared" si="2"/>
         <v>1465.0686361420001</v>
       </c>
-      <c r="F15" s="1">
+      <c r="F15" s="5">
         <v>-94726123.712203905</v>
       </c>
       <c r="G15" s="4">
         <f t="shared" si="3"/>
         <v>1440.016250655</v>
       </c>
-      <c r="H15" s="1">
+      <c r="H15" s="5">
         <v>-93337524.068543494</v>
       </c>
       <c r="I15" s="4">
@@ -12958,7 +12664,7 @@
         <f t="shared" si="6"/>
         <v>1.2798099055786754</v>
       </c>
-      <c r="M15" s="1">
+      <c r="M15">
         <v>996.02530587800004</v>
       </c>
       <c r="N15">
@@ -12979,21 +12685,21 @@
         <f t="shared" si="1"/>
         <v>1550.8148436910001</v>
       </c>
-      <c r="D16" s="1">
+      <c r="D16" s="5">
         <v>-92574367.957879007</v>
       </c>
       <c r="E16" s="4">
         <f t="shared" si="2"/>
         <v>1547.2598677210001</v>
       </c>
-      <c r="F16" s="1">
+      <c r="F16" s="5">
         <v>-94327686.7171406</v>
       </c>
       <c r="G16" s="4">
         <f t="shared" si="3"/>
         <v>1521.4672203540001</v>
       </c>
-      <c r="H16" s="1">
+      <c r="H16" s="5">
         <v>-92901458.871725202</v>
       </c>
       <c r="I16" s="4">
@@ -13012,7 +12718,7 @@
         <f t="shared" si="6"/>
         <v>1.2858171369520464</v>
       </c>
-      <c r="M16" s="1">
+      <c r="M16">
         <v>1079.98555259</v>
       </c>
       <c r="N16">
@@ -13033,21 +12739,21 @@
         <f t="shared" si="1"/>
         <v>1634.605218963</v>
       </c>
-      <c r="D17" s="1">
+      <c r="D17" s="5">
         <v>-92252325.532340199</v>
       </c>
       <c r="E17" s="4">
         <f t="shared" si="2"/>
         <v>1630.084266525</v>
       </c>
-      <c r="F17" s="1">
+      <c r="F17" s="5">
         <v>-93901256.2076502</v>
       </c>
       <c r="G17" s="4">
         <f t="shared" si="3"/>
         <v>1599.753059764</v>
       </c>
-      <c r="H17" s="1">
+      <c r="H17" s="5">
         <v>-92627683.177303493</v>
       </c>
       <c r="I17" s="4">
@@ -13066,7 +12772,7 @@
         <f t="shared" si="6"/>
         <v>1.289617571848972</v>
       </c>
-      <c r="M17" s="1">
+      <c r="M17">
         <v>1163.7759278619999</v>
       </c>
       <c r="N17">
@@ -13087,21 +12793,21 @@
         <f t="shared" si="1"/>
         <v>1718.189137439</v>
       </c>
-      <c r="D18" s="1">
+      <c r="D18" s="5">
         <v>-92025180.244919598</v>
       </c>
       <c r="E18" s="4">
         <f t="shared" si="2"/>
         <v>1712.3282496640002</v>
       </c>
-      <c r="F18" s="1">
+      <c r="F18" s="5">
         <v>-93605618.161412299</v>
       </c>
       <c r="G18" s="4">
         <f t="shared" si="3"/>
         <v>1678.7042750630001</v>
       </c>
-      <c r="H18" s="1">
+      <c r="H18" s="5">
         <v>-92332208.498645499</v>
       </c>
       <c r="I18" s="4">
@@ -13120,7 +12826,7 @@
         <f t="shared" si="6"/>
         <v>1.2937445102578953</v>
       </c>
-      <c r="M18" s="1">
+      <c r="M18">
         <v>1247.3598463379999</v>
       </c>
       <c r="N18">
@@ -13141,21 +12847,21 @@
         <f t="shared" si="1"/>
         <v>1801.4684374390001</v>
       </c>
-      <c r="D19" s="1">
+      <c r="D19" s="5">
         <v>-91861443.385459706</v>
       </c>
       <c r="E19" s="4">
         <f t="shared" si="2"/>
         <v>1794.5524029810001</v>
       </c>
-      <c r="F19" s="1">
+      <c r="F19" s="5">
         <v>-93343080.204725996</v>
       </c>
       <c r="G19" s="4">
         <f t="shared" si="3"/>
         <v>1757.9740589330002</v>
       </c>
-      <c r="H19" s="1">
+      <c r="H19" s="5">
         <v>-92120761.525859997</v>
       </c>
       <c r="I19" s="4">
@@ -13195,21 +12901,21 @@
         <f t="shared" si="1"/>
         <v>1885.461750232</v>
       </c>
-      <c r="D20" s="1">
+      <c r="D20" s="5">
         <v>-91616426.618146703</v>
       </c>
       <c r="E20" s="4">
         <f t="shared" si="2"/>
         <v>1875.6185091900002</v>
       </c>
-      <c r="F20" s="1">
+      <c r="F20" s="5">
         <v>-93102372.607865393</v>
       </c>
       <c r="G20" s="4">
         <f t="shared" si="3"/>
         <v>1837.1941077160002</v>
       </c>
-      <c r="H20" s="1">
+      <c r="H20" s="5">
         <v>-91897273.583140701</v>
       </c>
       <c r="I20" s="4">
@@ -13249,21 +12955,21 @@
         <f t="shared" si="1"/>
         <v>1968.0594826220001</v>
       </c>
-      <c r="D21" s="1">
+      <c r="D21" s="5">
         <v>-91424148.328540504</v>
       </c>
       <c r="E21" s="4">
         <f t="shared" si="2"/>
         <v>1957.561353517</v>
       </c>
-      <c r="F21" s="1">
+      <c r="F21" s="5">
         <v>-92895441.810325399</v>
       </c>
       <c r="G21" s="4">
         <f t="shared" si="3"/>
         <v>1916.984856518</v>
       </c>
-      <c r="H21" s="1">
+      <c r="H21" s="5">
         <v>-91707472.1862811</v>
       </c>
       <c r="I21" s="4">
@@ -13303,21 +13009,21 @@
         <f t="shared" si="1"/>
         <v>2050.8400371170001</v>
       </c>
-      <c r="D22" s="1">
+      <c r="D22" s="5">
         <v>-91246441.031971395</v>
       </c>
       <c r="E22" s="4">
         <f t="shared" si="2"/>
         <v>2041.183612694</v>
       </c>
-      <c r="F22" s="1">
+      <c r="F22" s="5">
         <v>-92640912.448044196</v>
       </c>
       <c r="G22" s="4">
         <f t="shared" si="3"/>
         <v>1996.7796368950001</v>
       </c>
-      <c r="H22" s="1">
+      <c r="H22" s="5">
         <v>-91577408.210854694</v>
       </c>
       <c r="I22" s="4">
@@ -13357,21 +13063,21 @@
         <f t="shared" si="1"/>
         <v>2134.5578774999999</v>
       </c>
-      <c r="D23" s="1">
+      <c r="D23" s="5">
         <v>-91113556.008599997</v>
       </c>
       <c r="E23" s="4">
         <f t="shared" si="2"/>
         <v>2123.5936180630001</v>
       </c>
-      <c r="F23" s="1">
+      <c r="F23" s="5">
         <v>-92415651.223814502</v>
       </c>
       <c r="G23" s="4">
         <f t="shared" si="3"/>
         <v>2076.5907951839999</v>
       </c>
-      <c r="H23" s="1">
+      <c r="H23" s="5">
         <v>-91457168.219560698</v>
       </c>
       <c r="I23" s="4">
@@ -13411,21 +13117,21 @@
         <f t="shared" si="1"/>
         <v>2217.0942264790001</v>
       </c>
-      <c r="D24" s="1">
+      <c r="D24" s="5">
         <v>-90985646.626872405</v>
       </c>
       <c r="E24" s="4">
         <f t="shared" si="2"/>
         <v>2206.4871730959999</v>
       </c>
-      <c r="F24" s="1">
+      <c r="F24" s="5">
         <v>-92236497.698856294</v>
       </c>
       <c r="G24" s="4">
         <f t="shared" si="3"/>
         <v>2154.6522989929999</v>
       </c>
-      <c r="H24" s="1">
+      <c r="H24" s="5">
         <v>-91285514.081303</v>
       </c>
       <c r="I24" s="4">
@@ -13465,21 +13171,21 @@
         <f t="shared" si="1"/>
         <v>2300.6605143050001</v>
       </c>
-      <c r="D25" s="1">
+      <c r="D25" s="5">
         <v>-90913617.454955801</v>
       </c>
       <c r="E25" s="4">
         <f t="shared" si="2"/>
         <v>2289.1109955689999</v>
       </c>
-      <c r="F25" s="1">
+      <c r="F25" s="5">
         <v>-92111985.008208394</v>
       </c>
       <c r="G25" s="4">
         <f t="shared" si="3"/>
         <v>2235.2299283100001</v>
       </c>
-      <c r="H25" s="1">
+      <c r="H25" s="5">
         <v>-91180700.302552298</v>
       </c>
       <c r="I25" s="4">
@@ -13519,21 +13225,21 @@
         <f t="shared" si="1"/>
         <v>2384.417359179</v>
       </c>
-      <c r="D26" s="1">
+      <c r="D26" s="5">
         <v>-90747004.321954101</v>
       </c>
       <c r="E26" s="4">
         <f t="shared" si="2"/>
         <v>2370.3054756699999</v>
       </c>
-      <c r="F26" s="1">
+      <c r="F26" s="5">
         <v>-91971319.229208499</v>
       </c>
       <c r="G26" s="4">
         <f t="shared" si="3"/>
         <v>2314.5615879530001</v>
       </c>
-      <c r="H26" s="1">
+      <c r="H26" s="5">
         <v>-91080541.504713297</v>
       </c>
       <c r="I26" s="4">
@@ -13573,21 +13279,21 @@
         <f t="shared" si="1"/>
         <v>2467.7641144620002</v>
       </c>
-      <c r="D27" s="1">
+      <c r="D27" s="5">
         <v>-90632012.854453102</v>
       </c>
       <c r="E27" s="4">
         <f t="shared" si="2"/>
         <v>2451.983852372</v>
       </c>
-      <c r="F27" s="1">
+      <c r="F27" s="5">
         <v>-91907863.867265299</v>
       </c>
       <c r="G27" s="4">
         <f t="shared" si="3"/>
         <v>2392.3100207809998</v>
       </c>
-      <c r="H27" s="1">
+      <c r="H27" s="5">
         <v>-90980785.130707502</v>
       </c>
       <c r="I27" s="4">
@@ -13627,21 +13333,21 @@
         <f t="shared" si="1"/>
         <v>2550.8223823939998</v>
       </c>
-      <c r="D28" s="1">
+      <c r="D28" s="5">
         <v>-90562102.780406594</v>
       </c>
       <c r="E28" s="4">
         <f t="shared" si="2"/>
         <v>2535.2788904109998</v>
       </c>
-      <c r="F28" s="1">
+      <c r="F28" s="5">
         <v>-91753542.326170504</v>
       </c>
       <c r="G28" s="4">
         <f t="shared" si="3"/>
         <v>2472.80892567</v>
       </c>
-      <c r="H28" s="1">
+      <c r="H28" s="5">
         <v>-90924626.747164294</v>
       </c>
       <c r="I28" s="4">
@@ -13681,21 +13387,21 @@
         <f t="shared" si="1"/>
         <v>2634.2359680909999</v>
       </c>
-      <c r="D29" s="1">
+      <c r="D29" s="5">
         <v>-90499309.651585102</v>
       </c>
       <c r="E29" s="4">
         <f t="shared" si="2"/>
         <v>2618.208308322</v>
       </c>
-      <c r="F29" s="1">
+      <c r="F29" s="5">
         <v>-91713476.7495085</v>
       </c>
       <c r="G29" s="4">
         <f t="shared" si="3"/>
         <v>2553.6312795959998</v>
       </c>
-      <c r="H29" s="1">
+      <c r="H29" s="5">
         <v>-90828735.012030393</v>
       </c>
       <c r="I29" s="4">
@@ -13735,21 +13441,21 @@
         <f t="shared" si="1"/>
         <v>2718.109388073</v>
       </c>
-      <c r="D30" s="1">
+      <c r="D30" s="5">
         <v>-90411475.893709406</v>
       </c>
       <c r="E30" s="4">
         <f t="shared" si="2"/>
         <v>2700.3606395289999</v>
       </c>
-      <c r="F30" s="1">
+      <c r="F30" s="5">
         <v>-91594311.868824601</v>
       </c>
       <c r="G30" s="4">
         <f t="shared" si="3"/>
         <v>2632.6519631629999</v>
       </c>
-      <c r="H30" s="1">
+      <c r="H30" s="5">
         <v>-90775404.439298794</v>
       </c>
       <c r="I30" s="4">
@@ -13789,21 +13495,21 @@
         <f t="shared" si="1"/>
         <v>2802.3509655899998</v>
       </c>
-      <c r="D31" s="1">
+      <c r="D31" s="5">
         <v>-90331746.249465302</v>
       </c>
       <c r="E31" s="4">
         <f t="shared" si="2"/>
         <v>2782.8122062839998</v>
       </c>
-      <c r="F31" s="1">
+      <c r="F31" s="5">
         <v>-91512211.550109804</v>
       </c>
       <c r="G31" s="4">
         <f t="shared" si="3"/>
         <v>2712.5687731539997</v>
       </c>
-      <c r="H31" s="1">
+      <c r="H31" s="5">
         <v>-90718062.162510604</v>
       </c>
       <c r="I31" s="4">
@@ -13843,24 +13549,24 @@
         <f t="shared" si="1"/>
         <v>2885.8088644579998</v>
       </c>
-      <c r="D32" s="1">
+      <c r="D32" s="5">
         <v>-90274495.947345898</v>
       </c>
       <c r="E32" s="4">
         <f t="shared" si="2"/>
         <v>2865.2995789279998</v>
       </c>
-      <c r="F32" s="1">
+      <c r="F32" s="5">
         <v>-91431225.932345107</v>
       </c>
       <c r="G32" s="4">
         <f t="shared" si="3"/>
         <v>2791.4172471349998</v>
       </c>
-      <c r="H32" s="1">
+      <c r="H32" s="5">
         <v>-90635230.365651101</v>
       </c>
-      <c r="I32" s="4"/>
+      <c r="I32" s="1"/>
       <c r="J32" s="4">
         <f t="shared" si="4"/>
         <v>1.3232340608668001</v>
@@ -13884,30 +13590,30 @@
       </c>
     </row>
     <row r="33" spans="1:15">
-      <c r="A33" s="4"/>
-      <c r="B33" s="5"/>
+      <c r="A33" s="1"/>
+      <c r="B33" s="1"/>
       <c r="C33" s="4">
         <f t="shared" si="1"/>
         <v>2970.379844648</v>
       </c>
-      <c r="D33" s="1">
+      <c r="D33" s="5">
         <v>-90173476.457734197</v>
       </c>
       <c r="E33" s="4">
         <f t="shared" si="2"/>
         <v>2947.4829306219999</v>
       </c>
-      <c r="F33" s="1">
+      <c r="F33" s="5">
         <v>-91308321.490612596</v>
       </c>
       <c r="G33" s="4">
         <f t="shared" si="3"/>
         <v>2870.431577412</v>
       </c>
-      <c r="H33" s="1">
+      <c r="H33" s="5">
         <v>-90603165.555318296</v>
       </c>
-      <c r="I33" s="4"/>
+      <c r="I33" s="1"/>
       <c r="J33" s="4">
         <f t="shared" si="4"/>
         <v>1.3247164527487214</v>
@@ -13931,30 +13637,30 @@
       </c>
     </row>
     <row r="34" spans="1:15">
-      <c r="A34" s="4"/>
-      <c r="B34" s="5"/>
+      <c r="A34" s="1"/>
+      <c r="B34" s="1"/>
       <c r="C34" s="4">
         <f t="shared" si="1"/>
         <v>3053.853088412</v>
       </c>
-      <c r="D34" s="1">
+      <c r="D34" s="5">
         <v>-90110578.638800204</v>
       </c>
       <c r="E34" s="4">
         <f t="shared" si="2"/>
         <v>3031.1270316109999</v>
       </c>
-      <c r="F34" s="1">
+      <c r="F34" s="5">
         <v>-91216653.012949303</v>
       </c>
       <c r="G34" s="4">
         <f t="shared" si="3"/>
         <v>2949.5303904809998</v>
       </c>
-      <c r="H34" s="1">
+      <c r="H34" s="5">
         <v>-90550342.280646205</v>
       </c>
-      <c r="I34" s="4"/>
+      <c r="I34" s="1"/>
       <c r="J34" s="4">
         <f t="shared" si="4"/>
         <v>1.3256411141685296</v>
@@ -13978,30 +13684,30 @@
       </c>
     </row>
     <row r="35" spans="1:15">
-      <c r="A35" s="4"/>
-      <c r="B35" s="5"/>
+      <c r="A35" s="1"/>
+      <c r="B35" s="1"/>
       <c r="C35" s="4">
         <f t="shared" si="1"/>
         <v>3136.0251260269997</v>
       </c>
-      <c r="D35" s="1">
+      <c r="D35" s="5">
         <v>-90054516.227057695</v>
       </c>
       <c r="E35" s="4">
         <f t="shared" si="2"/>
         <v>3113.4314331</v>
       </c>
-      <c r="F35" s="1">
+      <c r="F35" s="5">
         <v>-91172137.6546022</v>
       </c>
       <c r="G35" s="4">
         <f t="shared" si="3"/>
         <v>3028.9383100779996</v>
       </c>
-      <c r="H35" s="1">
+      <c r="H35" s="5">
         <v>-90502110.660838202</v>
       </c>
-      <c r="I35" s="4"/>
+      <c r="I35" s="1"/>
       <c r="J35" s="4">
         <f t="shared" si="4"/>
         <v>1.3264663769213483</v>
@@ -14025,30 +13731,30 @@
       </c>
     </row>
     <row r="36" spans="1:15">
-      <c r="A36" s="4"/>
-      <c r="B36" s="5"/>
+      <c r="A36" s="1"/>
+      <c r="B36" s="1"/>
       <c r="C36" s="4">
         <f t="shared" si="1"/>
         <v>3222.151921395</v>
       </c>
-      <c r="D36" s="1">
+      <c r="D36" s="5">
         <v>-89952531.676862001</v>
       </c>
       <c r="E36" s="4">
         <f t="shared" si="2"/>
         <v>3212.1519313109998</v>
       </c>
-      <c r="F36" s="1">
+      <c r="F36" s="5">
         <v>-91088271.810562894</v>
       </c>
       <c r="G36" s="4">
         <f t="shared" si="3"/>
         <v>3108.2972087319999</v>
       </c>
-      <c r="H36" s="1">
+      <c r="H36" s="5">
         <v>-90460026.320868298</v>
       </c>
-      <c r="I36" s="4"/>
+      <c r="I36" s="1"/>
       <c r="J36" s="4">
         <f t="shared" si="4"/>
         <v>1.3279702709672214</v>
@@ -14072,30 +13778,30 @@
       </c>
     </row>
     <row r="37" spans="1:15">
-      <c r="A37" s="4"/>
-      <c r="B37" s="5"/>
+      <c r="A37" s="1"/>
+      <c r="B37" s="1"/>
       <c r="C37" s="4">
         <f t="shared" si="1"/>
         <v>3305.6409161389997</v>
       </c>
-      <c r="D37" s="1">
+      <c r="D37" s="5">
         <v>-89920376.485272706</v>
       </c>
       <c r="E37" s="4">
         <f t="shared" si="2"/>
         <v>3296.0794084459999</v>
       </c>
-      <c r="F37" s="1">
+      <c r="F37" s="5">
         <v>-91042022.890332296</v>
       </c>
       <c r="G37" s="4">
         <f t="shared" si="3"/>
         <v>3194.2775188840001</v>
       </c>
-      <c r="H37" s="1">
+      <c r="H37" s="5">
         <v>-90416385.910040393</v>
       </c>
-      <c r="I37" s="4"/>
+      <c r="I37" s="1"/>
       <c r="J37" s="4">
         <f t="shared" si="4"/>
         <v>1.3284451481881239</v>
@@ -14119,30 +13825,30 @@
       </c>
     </row>
     <row r="38" spans="1:15">
-      <c r="A38" s="4"/>
-      <c r="B38" s="5"/>
+      <c r="A38" s="1"/>
+      <c r="B38" s="1"/>
       <c r="C38" s="4">
         <f t="shared" si="1"/>
         <v>3389.4199862400001</v>
       </c>
-      <c r="D38" s="1">
+      <c r="D38" s="5">
         <v>-89895213.486422896</v>
       </c>
       <c r="E38" s="4">
         <f t="shared" si="2"/>
         <v>3382.3357503669999</v>
       </c>
-      <c r="F38" s="1">
+      <c r="F38" s="5">
         <v>-90950571.165016994</v>
       </c>
       <c r="G38" s="4">
         <f t="shared" si="3"/>
         <v>3272.7951167739998</v>
       </c>
-      <c r="H38" s="1">
+      <c r="H38" s="5">
         <v>-90377002.103293598</v>
       </c>
-      <c r="I38" s="4"/>
+      <c r="I38" s="1"/>
       <c r="J38" s="4">
         <f t="shared" si="4"/>
         <v>1.3288169996186892</v>
@@ -14166,30 +13872,30 @@
       </c>
     </row>
     <row r="39" spans="1:15">
-      <c r="A39" s="4"/>
-      <c r="B39" s="5"/>
+      <c r="A39" s="1"/>
+      <c r="B39" s="1"/>
       <c r="C39" s="4">
         <f t="shared" si="1"/>
         <v>3472.9513212659999</v>
       </c>
-      <c r="D39" s="1">
+      <c r="D39" s="5">
         <v>-89840306.502251998</v>
       </c>
       <c r="E39" s="4">
         <f t="shared" si="2"/>
         <v>3465.331810483</v>
       </c>
-      <c r="F39" s="1">
+      <c r="F39" s="5">
         <v>-90844541.034822494</v>
       </c>
       <c r="G39" s="4">
         <f t="shared" si="3"/>
         <v>3352.8863482319998</v>
       </c>
-      <c r="H39" s="1">
+      <c r="H39" s="5">
         <v>-90349229.653967693</v>
       </c>
-      <c r="I39" s="4"/>
+      <c r="I39" s="1"/>
       <c r="J39" s="4">
         <f t="shared" si="4"/>
         <v>1.3296291221147567</v>
@@ -14213,30 +13919,30 @@
       </c>
     </row>
     <row r="40" spans="1:15">
-      <c r="A40" s="4"/>
-      <c r="B40" s="5"/>
+      <c r="A40" s="1"/>
+      <c r="B40" s="1"/>
       <c r="C40" s="4">
         <f t="shared" si="1"/>
         <v>3556.5380054449997</v>
       </c>
-      <c r="D40" s="1">
+      <c r="D40" s="5">
         <v>-89803131.211364403</v>
       </c>
       <c r="E40" s="4">
         <f t="shared" si="2"/>
         <v>3546.4818244459998</v>
       </c>
-      <c r="F40" s="1">
+      <c r="F40" s="5">
         <v>-90772653.197180703</v>
       </c>
       <c r="G40" s="4">
         <f t="shared" si="3"/>
         <v>3432.7087004679997</v>
       </c>
-      <c r="H40" s="1">
+      <c r="H40" s="5">
         <v>-90296995.681158006</v>
       </c>
-      <c r="I40" s="4"/>
+      <c r="I40" s="1"/>
       <c r="J40" s="4">
         <f t="shared" si="4"/>
         <v>1.3301795411115163</v>
@@ -14260,30 +13966,30 @@
       </c>
     </row>
     <row r="41" spans="1:15">
-      <c r="A41" s="4"/>
-      <c r="B41" s="5"/>
+      <c r="A41" s="1"/>
+      <c r="B41" s="1"/>
       <c r="C41" s="4">
         <f t="shared" si="1"/>
         <v>3638.8984410210001</v>
       </c>
-      <c r="D41" s="1">
+      <c r="D41" s="5">
         <v>-89781974.895667002</v>
       </c>
       <c r="E41" s="4">
         <f t="shared" si="2"/>
         <v>3628.5422157939997</v>
       </c>
-      <c r="F41" s="1">
+      <c r="F41" s="5">
         <v>-90734150.509338006</v>
       </c>
       <c r="G41" s="4">
         <f t="shared" si="3"/>
         <v>3512.8567436199996</v>
       </c>
-      <c r="H41" s="1">
+      <c r="H41" s="5">
         <v>-90267782.306004301</v>
       </c>
-      <c r="I41" s="4"/>
+      <c r="I41" s="1"/>
       <c r="J41" s="4">
         <f t="shared" si="4"/>
         <v>1.3304929859687795</v>
@@ -14307,30 +14013,30 @@
       </c>
     </row>
     <row r="42" spans="1:15">
-      <c r="A42" s="4"/>
-      <c r="B42" s="5"/>
+      <c r="A42" s="1"/>
+      <c r="B42" s="1"/>
       <c r="C42" s="4">
         <f t="shared" si="1"/>
         <v>3722.1820765359998</v>
       </c>
-      <c r="D42" s="1">
+      <c r="D42" s="5">
         <v>-89745322.671572998</v>
       </c>
       <c r="E42" s="4">
         <f t="shared" si="2"/>
         <v>3709.9335675839998</v>
       </c>
-      <c r="F42" s="1">
+      <c r="F42" s="5">
         <v>-90685886.196047395</v>
       </c>
       <c r="G42" s="4">
         <f t="shared" si="3"/>
         <v>3592.354784015</v>
       </c>
-      <c r="H42" s="1">
+      <c r="H42" s="5">
         <v>-90249985.873389706</v>
       </c>
-      <c r="I42" s="4"/>
+      <c r="I42" s="1"/>
       <c r="J42" s="4">
         <f t="shared" si="4"/>
         <v>1.3310363627780166</v>
@@ -14354,30 +14060,30 @@
       </c>
     </row>
     <row r="43" spans="1:15">
-      <c r="A43" s="4"/>
-      <c r="B43" s="5"/>
+      <c r="A43" s="1"/>
+      <c r="B43" s="1"/>
       <c r="C43" s="4">
         <f t="shared" si="1"/>
         <v>3805.2785085259998</v>
       </c>
-      <c r="D43" s="1">
+      <c r="D43" s="5">
         <v>-89714274.074118495</v>
       </c>
       <c r="E43" s="4">
         <f t="shared" si="2"/>
         <v>3792.0777554209999</v>
       </c>
-      <c r="F43" s="1">
+      <c r="F43" s="5">
         <v>-90671675.552113593</v>
       </c>
       <c r="G43" s="4">
         <f t="shared" si="3"/>
         <v>3673.6903734019998</v>
       </c>
-      <c r="H43" s="1">
+      <c r="H43" s="5">
         <v>-90215696.165335193</v>
       </c>
-      <c r="I43" s="4"/>
+      <c r="I43" s="1"/>
       <c r="J43" s="4">
         <f t="shared" si="4"/>
         <v>1.3314970120186387</v>
@@ -14401,30 +14107,30 @@
       </c>
     </row>
     <row r="44" spans="1:15">
-      <c r="A44" s="4"/>
-      <c r="B44" s="5"/>
+      <c r="A44" s="1"/>
+      <c r="B44" s="1"/>
       <c r="C44" s="4">
         <f t="shared" si="1"/>
         <v>3886.8073438389997</v>
       </c>
-      <c r="D44" s="1">
+      <c r="D44" s="5">
         <v>-89681867.861162901</v>
       </c>
       <c r="E44" s="4">
         <f t="shared" si="2"/>
         <v>3874.806601448</v>
       </c>
-      <c r="F44" s="1">
+      <c r="F44" s="5">
         <v>-90642747.446579695</v>
       </c>
       <c r="G44" s="4">
         <f t="shared" si="3"/>
         <v>3753.7334078109998</v>
       </c>
-      <c r="H44" s="1">
+      <c r="H44" s="5">
         <v>-90184875.121711597</v>
       </c>
-      <c r="I44" s="4"/>
+      <c r="I44" s="1"/>
       <c r="J44" s="4">
         <f t="shared" si="4"/>
         <v>1.3319781435645159</v>
@@ -14448,30 +14154,30 @@
       </c>
     </row>
     <row r="45" spans="1:15">
-      <c r="A45" s="4"/>
-      <c r="B45" s="5"/>
+      <c r="A45" s="1"/>
+      <c r="B45" s="1"/>
       <c r="C45" s="4">
         <f t="shared" si="1"/>
         <v>3969.8159261839996</v>
       </c>
-      <c r="D45" s="1">
+      <c r="D45" s="5">
         <v>-89630189.880454496</v>
       </c>
       <c r="E45" s="4">
         <f t="shared" si="2"/>
         <v>3957.6044917459999</v>
       </c>
-      <c r="F45" s="1">
+      <c r="F45" s="5">
         <v>-90607680.238301098</v>
       </c>
       <c r="G45" s="4">
         <f t="shared" si="3"/>
         <v>3832.5629442909999</v>
       </c>
-      <c r="H45" s="1">
+      <c r="H45" s="5">
         <v>-90156961.499264702</v>
       </c>
-      <c r="I45" s="4"/>
+      <c r="I45" s="1"/>
       <c r="J45" s="4">
         <f t="shared" si="4"/>
         <v>1.3327461207483082</v>
@@ -14495,30 +14201,30 @@
       </c>
     </row>
     <row r="46" spans="1:15">
-      <c r="A46" s="4"/>
-      <c r="B46" s="5"/>
+      <c r="A46" s="1"/>
+      <c r="B46" s="1"/>
       <c r="C46" s="4">
         <f t="shared" si="1"/>
         <v>4053.532168361</v>
       </c>
-      <c r="D46" s="1">
+      <c r="D46" s="5">
         <v>-89582289.650929898</v>
       </c>
       <c r="E46" s="4">
         <f t="shared" si="2"/>
         <v>4038.6787588769998</v>
       </c>
-      <c r="F46" s="1">
+      <c r="F46" s="5">
         <v>-90560758.920310795</v>
       </c>
       <c r="G46" s="4">
         <f t="shared" si="3"/>
         <v>3913.4285870379999</v>
       </c>
-      <c r="H46" s="1">
+      <c r="H46" s="5">
         <v>-90142283.546774805</v>
       </c>
-      <c r="I46" s="4"/>
+      <c r="I46" s="1"/>
       <c r="J46" s="4">
         <f t="shared" si="4"/>
         <v>1.3334587487167451</v>
@@ -14542,881 +14248,347 @@
       </c>
     </row>
     <row r="47" spans="1:15">
-      <c r="A47" s="4"/>
-      <c r="B47" s="5"/>
-      <c r="C47" s="4">
-        <f t="shared" si="1"/>
-        <v>4136.6838220099999</v>
-      </c>
-      <c r="D47" s="1">
-        <v>-89567726.327783093</v>
-      </c>
-      <c r="E47" s="4">
-        <f t="shared" si="2"/>
-        <v>4121.195089152</v>
-      </c>
-      <c r="F47" s="1">
-        <v>-90529087.747448295</v>
-      </c>
+      <c r="A47" s="1"/>
+      <c r="B47" s="1"/>
+      <c r="C47" s="1"/>
+      <c r="D47" s="1"/>
+      <c r="E47" s="1"/>
+      <c r="F47" s="1"/>
       <c r="G47" s="4">
         <f t="shared" si="3"/>
         <v>3995.0647215409999</v>
       </c>
-      <c r="H47" s="1">
+      <c r="H47" s="5">
         <v>-90115713.166437998</v>
       </c>
-      <c r="I47" s="4"/>
-      <c r="J47" s="4">
-        <f t="shared" si="4"/>
-        <v>1.3336755633156712</v>
-      </c>
-      <c r="K47" s="4">
-        <f t="shared" si="5"/>
-        <v>1.3195127758091985</v>
-      </c>
+      <c r="I47" s="1"/>
+      <c r="J47" s="1"/>
+      <c r="K47" s="1"/>
       <c r="L47" s="4">
         <f t="shared" si="6"/>
         <v>1.3255655830463831</v>
       </c>
-      <c r="M47">
-        <v>3665.854530909</v>
-      </c>
-      <c r="N47">
-        <v>3650.3657980510002</v>
-      </c>
       <c r="O47">
         <v>3524.2354304400001</v>
       </c>
     </row>
     <row r="48" spans="1:15">
-      <c r="A48" s="4"/>
-      <c r="B48" s="5"/>
-      <c r="C48" s="4">
-        <f t="shared" si="1"/>
-        <v>4220.8108135689999</v>
-      </c>
-      <c r="D48" s="1">
-        <v>-89528975.862185195</v>
-      </c>
-      <c r="E48" s="4">
-        <f t="shared" si="2"/>
-        <v>4202.8121536890003</v>
-      </c>
-      <c r="F48" s="1">
-        <v>-90484305.971721202</v>
-      </c>
+      <c r="A48" s="1"/>
+      <c r="B48" s="1"/>
+      <c r="C48" s="1"/>
+      <c r="D48" s="1"/>
+      <c r="E48" s="1"/>
+      <c r="F48" s="1"/>
       <c r="G48" s="4">
         <f t="shared" si="3"/>
         <v>4074.4336242149998</v>
       </c>
-      <c r="H48" s="1">
+      <c r="H48" s="5">
         <v>-90104318.703545198</v>
       </c>
-      <c r="I48" s="4"/>
-      <c r="J48" s="4">
-        <f t="shared" si="4"/>
-        <v>1.3342528127317104</v>
-      </c>
-      <c r="K48" s="4">
-        <f t="shared" si="5"/>
-        <v>1.3201658186165752</v>
-      </c>
+      <c r="I48" s="1"/>
+      <c r="J48" s="1"/>
+      <c r="K48" s="1"/>
       <c r="L48" s="4">
         <f t="shared" si="6"/>
         <v>1.325733212168553</v>
       </c>
-      <c r="M48">
-        <v>3749.9815224680001</v>
-      </c>
-      <c r="N48">
-        <v>3731.982862588</v>
-      </c>
       <c r="O48">
         <v>3603.6043331139999</v>
       </c>
     </row>
-    <row r="49" spans="1:15">
-      <c r="A49" s="4"/>
-      <c r="B49" s="5"/>
-      <c r="C49" s="4">
-        <f t="shared" si="1"/>
-        <v>4303.9453012350004</v>
-      </c>
-      <c r="D49" s="1">
-        <v>-89499615.291737303</v>
-      </c>
-      <c r="E49" s="4">
-        <f t="shared" si="2"/>
-        <v>4285.8016599290004</v>
-      </c>
-      <c r="F49" s="1">
-        <v>-90469576.553930998</v>
-      </c>
-      <c r="G49" s="4">
-        <f t="shared" si="3"/>
-        <v>4153.5122264510001</v>
-      </c>
-      <c r="H49" s="1">
-        <v>-90080595.295350194</v>
-      </c>
-      <c r="I49" s="4"/>
-      <c r="J49" s="4">
-        <f t="shared" si="4"/>
-        <v>1.3346905176712882</v>
-      </c>
-      <c r="K49" s="4">
-        <f t="shared" si="5"/>
-        <v>1.3203807557770599</v>
-      </c>
-      <c r="L49" s="4">
-        <f t="shared" si="6"/>
-        <v>1.3260823540680577</v>
-      </c>
-      <c r="M49">
-        <v>3833.1160101340001</v>
-      </c>
-      <c r="N49">
-        <v>3814.9723688280001</v>
-      </c>
-      <c r="O49">
-        <v>3682.6829353500002</v>
-      </c>
-    </row>
-    <row r="50" spans="1:15">
-      <c r="A50" s="4"/>
-      <c r="B50" s="5"/>
-      <c r="C50" s="4">
-        <f t="shared" si="1"/>
-        <v>4385.917480131</v>
-      </c>
-      <c r="D50" s="1">
-        <v>-89473778.653625399</v>
-      </c>
-      <c r="E50" s="4">
-        <f t="shared" si="2"/>
-        <v>4367.6219745690005</v>
-      </c>
-      <c r="F50" s="1">
-        <v>-90450371.5051305</v>
-      </c>
-      <c r="G50" s="4">
-        <f t="shared" si="3"/>
-        <v>4232.5376109280005</v>
-      </c>
-      <c r="H50" s="1">
-        <v>-90065223.292657793</v>
-      </c>
-      <c r="I50" s="4"/>
-      <c r="J50" s="4">
-        <f t="shared" si="4"/>
-        <v>1.3350759257362583</v>
-      </c>
-      <c r="K50" s="4">
-        <f t="shared" si="5"/>
-        <v>1.3206611081562483</v>
-      </c>
-      <c r="L50" s="4">
-        <f t="shared" si="6"/>
-        <v>1.3263086849510761</v>
-      </c>
-      <c r="M50">
-        <v>3915.0881890300002</v>
-      </c>
-      <c r="N50">
-        <v>3896.7926834680002</v>
-      </c>
-      <c r="O50">
-        <v>3761.7083198270002</v>
-      </c>
-    </row>
-    <row r="51" spans="1:15">
-      <c r="A51" s="4"/>
-      <c r="B51" s="5"/>
-      <c r="C51" s="4">
-        <f t="shared" si="1"/>
-        <v>4469.1083906949998</v>
-      </c>
-      <c r="D51" s="1">
-        <v>-89465261.991689995</v>
-      </c>
-      <c r="E51" s="4">
-        <f t="shared" si="2"/>
-        <v>4450.1061130179996</v>
-      </c>
-      <c r="F51" s="1">
-        <v>-90402601.200713396</v>
-      </c>
-      <c r="G51" s="4">
-        <f t="shared" si="3"/>
-        <v>4313.8074758889998</v>
-      </c>
-      <c r="H51" s="1">
-        <v>-90033911.277243599</v>
-      </c>
-      <c r="I51" s="4"/>
-      <c r="J51" s="4">
-        <f t="shared" si="4"/>
-        <v>1.3352030185325512</v>
-      </c>
-      <c r="K51" s="4">
-        <f t="shared" si="5"/>
-        <v>1.3213589684205607</v>
-      </c>
-      <c r="L51" s="4">
-        <f t="shared" si="6"/>
-        <v>1.3267699489059352</v>
-      </c>
-      <c r="M51">
-        <v>3998.2790995939999</v>
-      </c>
-      <c r="N51">
-        <v>3979.2768219169998</v>
-      </c>
-      <c r="O51">
-        <v>3842.9781847879999</v>
-      </c>
-    </row>
-    <row r="52" spans="1:15">
-      <c r="A52" s="4"/>
-      <c r="B52" s="5"/>
-      <c r="C52" s="4">
-        <f t="shared" si="1"/>
-        <v>4552.900793191</v>
-      </c>
-      <c r="D52" s="1">
-        <v>-89444935.105609402</v>
-      </c>
-      <c r="E52" s="4">
-        <f t="shared" si="2"/>
-        <v>4532.9034727650005</v>
-      </c>
-      <c r="F52" s="1">
-        <v>-90337185.923213199</v>
-      </c>
-      <c r="G52" s="4">
-        <f t="shared" si="3"/>
-        <v>4393.3116127290004</v>
-      </c>
-      <c r="H52" s="1">
-        <v>-90012052.034714803</v>
-      </c>
-      <c r="I52" s="4"/>
-      <c r="J52" s="4">
-        <f t="shared" si="4"/>
-        <v>1.335506451249229</v>
-      </c>
-      <c r="K52" s="4">
-        <f t="shared" si="5"/>
-        <v>1.3223157954759228</v>
-      </c>
-      <c r="L52" s="4">
-        <f t="shared" si="6"/>
-        <v>1.3270921522713452</v>
-      </c>
-      <c r="M52">
-        <v>4082.0715020900002</v>
-      </c>
-      <c r="N52">
-        <v>4062.0741816640002</v>
-      </c>
-      <c r="O52">
-        <v>3922.4823216280001</v>
-      </c>
-    </row>
-    <row r="53" spans="1:15">
-      <c r="A53" s="4"/>
-      <c r="B53" s="5"/>
-      <c r="C53" s="4">
-        <f t="shared" si="1"/>
-        <v>4637.6446765540004</v>
-      </c>
-      <c r="D53" s="1">
-        <v>-89413264.937215298</v>
-      </c>
-      <c r="E53" s="4">
-        <f t="shared" si="2"/>
-        <v>4613.1927548350004</v>
-      </c>
-      <c r="F53" s="1">
-        <v>-90302465.600890204</v>
-      </c>
-      <c r="G53" s="4">
-        <f t="shared" si="3"/>
-        <v>4472.8892323560003</v>
-      </c>
-      <c r="H53" s="1">
-        <v>-89987586.830922604</v>
-      </c>
-      <c r="I53" s="4"/>
-      <c r="J53" s="4">
-        <f t="shared" si="4"/>
-        <v>1.3359794874842013</v>
-      </c>
-      <c r="K53" s="4">
-        <f t="shared" si="5"/>
-        <v>1.3228242116119187</v>
-      </c>
-      <c r="L53" s="4">
-        <f t="shared" si="6"/>
-        <v>1.3274529529228547</v>
-      </c>
-      <c r="M53">
-        <v>4166.8153854530001</v>
-      </c>
-      <c r="N53">
-        <v>4142.3634637340001</v>
-      </c>
-      <c r="O53">
-        <v>4002.059941255</v>
-      </c>
-    </row>
-    <row r="54" spans="1:15">
-      <c r="A54" s="4"/>
-      <c r="B54" s="5"/>
-      <c r="C54" s="4">
-        <f t="shared" si="1"/>
-        <v>4721.6336280430005</v>
-      </c>
-      <c r="D54" s="1">
-        <v>-89384172.043536395</v>
-      </c>
-      <c r="E54" s="4">
-        <f t="shared" si="2"/>
-        <v>4694.8549507200005</v>
-      </c>
-      <c r="F54" s="1">
-        <v>-90291140.140596807</v>
-      </c>
-      <c r="G54" s="4">
-        <f t="shared" si="3"/>
-        <v>4553.8964713980004</v>
-      </c>
-      <c r="H54" s="1">
-        <v>-89974479.685031101</v>
-      </c>
-      <c r="I54" s="4"/>
-      <c r="J54" s="4">
-        <f t="shared" si="4"/>
-        <v>1.3364143240810837</v>
-      </c>
-      <c r="K54" s="4">
-        <f t="shared" si="5"/>
-        <v>1.3229901370068182</v>
-      </c>
-      <c r="L54" s="4">
-        <f t="shared" si="6"/>
-        <v>1.3276463313072473</v>
-      </c>
-      <c r="M54">
-        <v>4250.8043369420002</v>
-      </c>
-      <c r="N54">
-        <v>4224.0256596190002</v>
-      </c>
-      <c r="O54">
-        <v>4083.067180297</v>
-      </c>
-    </row>
-    <row r="55" spans="1:15">
-      <c r="A55" s="4"/>
-      <c r="B55" s="5"/>
-      <c r="C55" s="4">
-        <f t="shared" si="1"/>
-        <v>4804.7717106310001</v>
-      </c>
-      <c r="D55" s="1">
-        <v>-89373282.3425349</v>
-      </c>
-      <c r="E55" s="4">
-        <f t="shared" si="2"/>
-        <v>4777.7773630830006</v>
-      </c>
-      <c r="F55" s="1">
-        <v>-90262546.139437899</v>
-      </c>
-      <c r="G55" s="4">
-        <f t="shared" si="3"/>
-        <v>4633.6961713569999</v>
-      </c>
-      <c r="H55" s="1">
-        <v>-89965384.331577897</v>
-      </c>
-      <c r="I55" s="4"/>
-      <c r="J55" s="4">
-        <f t="shared" si="4"/>
-        <v>1.3365771596849902</v>
-      </c>
-      <c r="K55" s="4">
-        <f t="shared" si="5"/>
-        <v>1.3234092430826911</v>
-      </c>
-      <c r="L55" s="4">
-        <f t="shared" si="6"/>
-        <v>1.3277805541834546</v>
-      </c>
-      <c r="M55">
-        <v>4333.9424195299998</v>
-      </c>
-      <c r="N55">
-        <v>4306.9480719820003</v>
-      </c>
-      <c r="O55">
-        <v>4162.8668802559996</v>
-      </c>
-    </row>
-    <row r="56" spans="1:15">
-      <c r="A56" s="4"/>
-      <c r="B56" s="5"/>
-      <c r="C56" s="4">
-        <f t="shared" si="1"/>
-        <v>4887.5379353560002</v>
-      </c>
-      <c r="D56" s="1">
-        <v>-89349907.271207705</v>
-      </c>
-      <c r="E56" s="4">
-        <f t="shared" si="2"/>
-        <v>4859.1491849560007</v>
-      </c>
-      <c r="F56" s="1">
-        <v>-90201980.842276394</v>
-      </c>
-      <c r="G56" s="4">
-        <f t="shared" si="3"/>
-        <v>4715.010542598</v>
-      </c>
-      <c r="H56" s="1">
-        <v>-89949221.935111195</v>
-      </c>
-      <c r="I56" s="4"/>
-      <c r="J56" s="4">
-        <f t="shared" si="4"/>
-        <v>1.3369268252570776</v>
-      </c>
-      <c r="K56" s="4">
-        <f t="shared" si="5"/>
-        <v>1.3242978341460485</v>
-      </c>
-      <c r="L56" s="4">
-        <f t="shared" si="6"/>
-        <v>1.3280191345210697</v>
-      </c>
-      <c r="M56">
-        <v>4416.7086442549999</v>
-      </c>
-      <c r="N56">
-        <v>4388.3198938550004</v>
-      </c>
-      <c r="O56">
-        <v>4244.1812514969997</v>
-      </c>
-    </row>
-    <row r="57" spans="1:15">
-      <c r="A57" s="4"/>
-      <c r="B57" s="5"/>
-      <c r="C57" s="4">
-        <f t="shared" si="1"/>
-        <v>4972.5253931610005</v>
-      </c>
-      <c r="D57" s="1">
-        <v>-89326098.716698796</v>
-      </c>
-      <c r="E57" s="4">
-        <f t="shared" si="2"/>
-        <v>4942.7563706629999</v>
-      </c>
-      <c r="F57" s="1">
-        <v>-90161545.367942005</v>
-      </c>
-      <c r="G57" s="4">
-        <f t="shared" si="3"/>
-        <v>4796.1915761340006</v>
-      </c>
-      <c r="H57" s="1">
-        <v>-89930825.466356695</v>
-      </c>
-      <c r="I57" s="4"/>
-      <c r="J57" s="4">
-        <f t="shared" si="4"/>
-        <v>1.337283163389503</v>
-      </c>
-      <c r="K57" s="4">
-        <f t="shared" si="5"/>
-        <v>1.3248917526604793</v>
-      </c>
-      <c r="L57" s="4">
-        <f t="shared" si="6"/>
-        <v>1.3282907973506601</v>
-      </c>
-      <c r="M57">
-        <v>4501.6961020600002</v>
-      </c>
-      <c r="N57">
-        <v>4471.9270795619996</v>
-      </c>
-      <c r="O57">
-        <v>4325.3622850330003</v>
-      </c>
-    </row>
-    <row r="58" spans="1:15">
-      <c r="A58" s="4"/>
-      <c r="B58" s="5"/>
-      <c r="C58" s="4">
-        <f t="shared" si="1"/>
-        <v>5056.4610624610004</v>
-      </c>
-      <c r="D58" s="1">
-        <v>-89309114.332913294</v>
-      </c>
-      <c r="E58" s="4">
-        <f t="shared" si="2"/>
-        <v>5025.4588759819999</v>
-      </c>
-      <c r="F58" s="1">
-        <v>-90143207.832639799</v>
-      </c>
-      <c r="G58" s="4">
-        <f t="shared" si="3"/>
-        <v>4876.5775772810002</v>
-      </c>
-      <c r="H58" s="1">
-        <v>-89916514.164873898</v>
-      </c>
-      <c r="I58" s="4"/>
-      <c r="J58" s="4">
-        <f t="shared" si="4"/>
-        <v>1.337537481559004</v>
-      </c>
-      <c r="K58" s="4">
-        <f t="shared" si="5"/>
-        <v>1.3251612710176595</v>
-      </c>
-      <c r="L58" s="4">
-        <f t="shared" si="6"/>
-        <v>1.3285022109072717</v>
-      </c>
-      <c r="M58">
-        <v>4585.6317713600001</v>
-      </c>
-      <c r="N58">
-        <v>4554.6295848809996</v>
-      </c>
-      <c r="O58">
-        <v>4405.7482861799999</v>
-      </c>
-    </row>
-    <row r="59" spans="1:15">
-      <c r="A59" s="4"/>
-      <c r="B59" s="5"/>
-      <c r="C59" s="4">
-        <f t="shared" si="1"/>
-        <v>5139.0853902460003</v>
-      </c>
-      <c r="D59" s="1">
-        <v>-89288907.848316297</v>
-      </c>
-      <c r="E59" s="4">
-        <f t="shared" si="2"/>
-        <v>5107.9131224110006</v>
-      </c>
-      <c r="F59" s="1">
-        <v>-90117634.231237203</v>
-      </c>
-      <c r="G59" s="4">
-        <f t="shared" si="3"/>
-        <v>4956.4144026690001</v>
-      </c>
-      <c r="H59" s="1">
-        <v>-89903626.322097898</v>
-      </c>
-      <c r="I59" s="4"/>
-      <c r="J59" s="4">
-        <f t="shared" si="4"/>
-        <v>1.3378401723542026</v>
-      </c>
-      <c r="K59" s="4">
-        <f t="shared" si="5"/>
-        <v>1.3255373255648994</v>
-      </c>
-      <c r="L59" s="4">
-        <f t="shared" si="6"/>
-        <v>1.3286926540331185</v>
-      </c>
-      <c r="M59">
-        <v>4668.256099145</v>
-      </c>
-      <c r="N59">
-        <v>4637.0838313100003</v>
-      </c>
-      <c r="O59">
-        <v>4485.5851115679998</v>
-      </c>
-    </row>
-    <row r="60" spans="1:15">
-      <c r="A60" s="4"/>
-      <c r="B60" s="5"/>
-      <c r="C60" s="4">
-        <f t="shared" si="1"/>
-        <v>5222.4662009510002</v>
-      </c>
-      <c r="D60" s="1">
-        <v>-89281763.362811595</v>
-      </c>
-      <c r="E60" s="4">
-        <f t="shared" si="2"/>
-        <v>5190.4899758490001</v>
-      </c>
-      <c r="F60" s="1">
-        <v>-90095809.791911796</v>
-      </c>
-      <c r="G60" s="4">
-        <f t="shared" si="3"/>
-        <v>5037.121045119</v>
-      </c>
-      <c r="H60" s="1">
-        <v>-89893031.370448694</v>
-      </c>
-      <c r="I60" s="4"/>
-      <c r="J60" s="4">
-        <f t="shared" si="4"/>
-        <v>1.3379472287043348</v>
-      </c>
-      <c r="K60" s="4">
-        <f t="shared" si="5"/>
-        <v>1.3258584182883255</v>
-      </c>
-      <c r="L60" s="4">
-        <f t="shared" si="6"/>
-        <v>1.3288492560990577</v>
-      </c>
-      <c r="M60">
-        <v>4751.6369098499999</v>
-      </c>
-      <c r="N60">
-        <v>4719.6606847479998</v>
-      </c>
-      <c r="O60">
-        <v>4566.2917540179997</v>
-      </c>
-    </row>
-    <row r="61" spans="1:15">
-      <c r="A61" s="4"/>
-      <c r="B61" s="5"/>
-      <c r="C61" s="4">
-        <f t="shared" si="1"/>
-        <v>5306.4956114420002</v>
-      </c>
-      <c r="D61" s="1">
-        <v>-89264932.745486498</v>
-      </c>
-      <c r="E61" s="4">
-        <f t="shared" si="2"/>
-        <v>5272.0316073070007</v>
-      </c>
-      <c r="F61" s="1">
-        <v>-90061417.241869703</v>
-      </c>
-      <c r="G61" s="4">
-        <f t="shared" si="3"/>
-        <v>5117.4880875830004</v>
-      </c>
-      <c r="H61" s="1">
-        <v>-89882899.639612705</v>
-      </c>
-      <c r="I61" s="4"/>
-      <c r="J61" s="4">
-        <f t="shared" si="4"/>
-        <v>1.3381994943714328</v>
-      </c>
-      <c r="K61" s="4">
-        <f t="shared" si="5"/>
-        <v>1.3263647355704224</v>
-      </c>
-      <c r="L61" s="4">
-        <f t="shared" si="6"/>
-        <v>1.3289990459148999</v>
-      </c>
-      <c r="M61">
-        <v>4835.6663203409998</v>
-      </c>
-      <c r="N61">
-        <v>4801.2023162060004</v>
-      </c>
-      <c r="O61">
-        <v>4646.6587964820001</v>
-      </c>
-    </row>
-    <row r="62" spans="1:15">
-      <c r="A62" s="4"/>
-      <c r="B62" s="5"/>
-      <c r="C62" s="4">
-        <f t="shared" si="1"/>
-        <v>5389.4706996069999</v>
-      </c>
-      <c r="D62" s="1">
-        <v>-89253237.087655902</v>
-      </c>
-      <c r="E62" s="4">
-        <f t="shared" si="2"/>
-        <v>5355.1373321810006</v>
-      </c>
-      <c r="F62" s="1">
-        <v>-90030730.155291095</v>
-      </c>
-      <c r="G62" s="4">
-        <f t="shared" si="3"/>
-        <v>5197.3630026179999</v>
-      </c>
-      <c r="H62" s="1">
-        <v>-89857589.736041203</v>
-      </c>
-      <c r="I62" s="4"/>
-      <c r="J62" s="4">
-        <f t="shared" si="4"/>
-        <v>1.3383748507383944</v>
-      </c>
-      <c r="K62" s="4">
-        <f t="shared" si="5"/>
-        <v>1.3268168286435882</v>
-      </c>
-      <c r="L62" s="4">
-        <f t="shared" si="6"/>
-        <v>1.3293733808797876</v>
-      </c>
-      <c r="M62">
-        <v>4918.6414085059996</v>
-      </c>
-      <c r="N62">
-        <v>4884.3080410800003</v>
-      </c>
-      <c r="O62">
-        <v>4726.5337115169996</v>
-      </c>
-    </row>
-    <row r="63" spans="1:15">
-      <c r="A63" s="4"/>
-      <c r="B63" s="5"/>
-      <c r="C63" s="5"/>
-      <c r="D63" s="5"/>
-      <c r="E63" s="4"/>
-      <c r="F63" s="5"/>
-      <c r="G63" s="4">
-        <f t="shared" si="3"/>
-        <v>5278.2189759130006</v>
-      </c>
-      <c r="H63" s="1">
-        <v>-89853080.026942</v>
-      </c>
-      <c r="I63" s="4"/>
-      <c r="J63" s="4"/>
-      <c r="K63" s="4"/>
-      <c r="L63" s="4">
-        <f t="shared" si="6"/>
-        <v>1.3294401018784467</v>
-      </c>
-      <c r="O63">
-        <v>4807.3896848120003</v>
-      </c>
-    </row>
-    <row r="64" spans="1:15">
-      <c r="A64" s="4"/>
-      <c r="B64" s="5"/>
-      <c r="C64" s="5"/>
-      <c r="D64" s="5"/>
-      <c r="E64" s="4"/>
-      <c r="F64" s="5"/>
-      <c r="G64" s="4">
-        <f t="shared" si="3"/>
-        <v>5359.5431572440002</v>
-      </c>
-      <c r="H64" s="1">
-        <v>-89847439.301113501</v>
-      </c>
-      <c r="I64" s="4"/>
-      <c r="J64" s="4"/>
-      <c r="K64" s="4"/>
-      <c r="L64" s="4">
-        <f t="shared" si="6"/>
-        <v>1.3295235656608142</v>
-      </c>
-      <c r="O64">
-        <v>4888.7138661429999</v>
-      </c>
+    <row r="49" spans="1:12">
+      <c r="A49" s="1"/>
+      <c r="B49" s="1"/>
+      <c r="C49" s="1"/>
+      <c r="D49" s="1"/>
+      <c r="E49" s="1"/>
+      <c r="F49" s="1"/>
+      <c r="G49" s="1"/>
+      <c r="H49" s="1"/>
+      <c r="I49" s="1"/>
+      <c r="J49" s="1"/>
+      <c r="K49" s="1"/>
+      <c r="L49" s="1"/>
+    </row>
+    <row r="50" spans="1:12">
+      <c r="A50" s="1"/>
+      <c r="B50" s="1"/>
+      <c r="C50" s="1"/>
+      <c r="D50" s="1"/>
+      <c r="E50" s="1"/>
+      <c r="F50" s="1"/>
+      <c r="G50" s="1"/>
+      <c r="H50" s="1"/>
+      <c r="I50" s="1"/>
+      <c r="J50" s="1"/>
+      <c r="K50" s="1"/>
+      <c r="L50" s="1"/>
+    </row>
+    <row r="51" spans="1:12">
+      <c r="A51" s="1"/>
+      <c r="B51" s="1"/>
+      <c r="C51" s="1"/>
+      <c r="D51" s="1"/>
+      <c r="E51" s="1"/>
+      <c r="F51" s="1"/>
+      <c r="G51" s="1"/>
+      <c r="H51" s="1"/>
+      <c r="I51" s="1"/>
+      <c r="J51" s="1"/>
+      <c r="K51" s="1"/>
+      <c r="L51" s="1"/>
+    </row>
+    <row r="52" spans="1:12">
+      <c r="A52" s="1"/>
+      <c r="B52" s="1"/>
+      <c r="C52" s="1"/>
+      <c r="D52" s="1"/>
+      <c r="E52" s="1"/>
+      <c r="F52" s="1"/>
+      <c r="G52" s="1"/>
+      <c r="H52" s="1"/>
+      <c r="I52" s="1"/>
+      <c r="J52" s="1"/>
+      <c r="K52" s="1"/>
+      <c r="L52" s="1"/>
+    </row>
+    <row r="53" spans="1:12">
+      <c r="A53" s="1"/>
+      <c r="B53" s="1"/>
+      <c r="C53" s="1"/>
+      <c r="D53" s="1"/>
+      <c r="E53" s="1"/>
+      <c r="F53" s="1"/>
+      <c r="G53" s="1"/>
+      <c r="H53" s="1"/>
+      <c r="I53" s="1"/>
+      <c r="J53" s="1"/>
+      <c r="K53" s="1"/>
+      <c r="L53" s="1"/>
+    </row>
+    <row r="54" spans="1:12">
+      <c r="A54" s="1"/>
+      <c r="B54" s="1"/>
+      <c r="C54" s="1"/>
+      <c r="D54" s="1"/>
+      <c r="E54" s="1"/>
+      <c r="F54" s="1"/>
+      <c r="G54" s="1"/>
+      <c r="H54" s="1"/>
+      <c r="I54" s="1"/>
+      <c r="J54" s="1"/>
+      <c r="K54" s="1"/>
+      <c r="L54" s="1"/>
+    </row>
+    <row r="55" spans="1:12">
+      <c r="A55" s="1"/>
+      <c r="B55" s="1"/>
+      <c r="C55" s="1"/>
+      <c r="D55" s="1"/>
+      <c r="E55" s="1"/>
+      <c r="F55" s="1"/>
+      <c r="G55" s="1"/>
+      <c r="H55" s="1"/>
+      <c r="I55" s="1"/>
+      <c r="J55" s="1"/>
+      <c r="K55" s="1"/>
+      <c r="L55" s="1"/>
+    </row>
+    <row r="56" spans="1:12">
+      <c r="A56" s="1"/>
+      <c r="B56" s="1"/>
+      <c r="C56" s="1"/>
+      <c r="D56" s="1"/>
+      <c r="E56" s="1"/>
+      <c r="F56" s="1"/>
+      <c r="G56" s="1"/>
+      <c r="H56" s="1"/>
+      <c r="I56" s="1"/>
+      <c r="J56" s="1"/>
+      <c r="K56" s="1"/>
+      <c r="L56" s="1"/>
+    </row>
+    <row r="57" spans="1:12">
+      <c r="A57" s="1"/>
+      <c r="B57" s="1"/>
+      <c r="C57" s="1"/>
+      <c r="D57" s="1"/>
+      <c r="E57" s="1"/>
+      <c r="F57" s="1"/>
+      <c r="G57" s="1"/>
+      <c r="H57" s="1"/>
+      <c r="I57" s="1"/>
+      <c r="J57" s="1"/>
+      <c r="K57" s="1"/>
+      <c r="L57" s="1"/>
+    </row>
+    <row r="58" spans="1:12">
+      <c r="A58" s="1"/>
+      <c r="B58" s="1"/>
+      <c r="C58" s="1"/>
+      <c r="D58" s="1"/>
+      <c r="E58" s="1"/>
+      <c r="F58" s="1"/>
+      <c r="G58" s="1"/>
+      <c r="H58" s="1"/>
+      <c r="I58" s="1"/>
+      <c r="J58" s="1"/>
+      <c r="K58" s="1"/>
+      <c r="L58" s="1"/>
+    </row>
+    <row r="59" spans="1:12">
+      <c r="A59" s="1"/>
+      <c r="B59" s="1"/>
+      <c r="C59" s="1"/>
+      <c r="D59" s="1"/>
+      <c r="E59" s="1"/>
+      <c r="F59" s="1"/>
+      <c r="G59" s="1"/>
+      <c r="H59" s="1"/>
+      <c r="I59" s="1"/>
+      <c r="J59" s="1"/>
+      <c r="K59" s="1"/>
+      <c r="L59" s="1"/>
+    </row>
+    <row r="60" spans="1:12">
+      <c r="A60" s="1"/>
+      <c r="B60" s="1"/>
+      <c r="C60" s="1"/>
+      <c r="D60" s="1"/>
+      <c r="E60" s="1"/>
+      <c r="F60" s="1"/>
+      <c r="G60" s="1"/>
+      <c r="H60" s="1"/>
+      <c r="I60" s="1"/>
+      <c r="J60" s="1"/>
+      <c r="K60" s="1"/>
+      <c r="L60" s="1"/>
+    </row>
+    <row r="61" spans="1:12">
+      <c r="A61" s="1"/>
+      <c r="B61" s="1"/>
+      <c r="C61" s="1"/>
+      <c r="D61" s="1"/>
+      <c r="E61" s="1"/>
+      <c r="F61" s="1"/>
+      <c r="G61" s="1"/>
+      <c r="H61" s="1"/>
+      <c r="I61" s="1"/>
+      <c r="J61" s="1"/>
+      <c r="K61" s="1"/>
+      <c r="L61" s="1"/>
+    </row>
+    <row r="62" spans="1:12">
+      <c r="A62" s="1"/>
+      <c r="B62" s="1"/>
+      <c r="C62" s="1"/>
+      <c r="D62" s="1"/>
+      <c r="E62" s="1"/>
+      <c r="F62" s="1"/>
+      <c r="G62" s="1"/>
+      <c r="H62" s="1"/>
+      <c r="I62" s="1"/>
+      <c r="J62" s="1"/>
+      <c r="K62" s="1"/>
+      <c r="L62" s="1"/>
+    </row>
+    <row r="63" spans="1:12">
+      <c r="A63" s="1"/>
+      <c r="B63" s="1"/>
+      <c r="C63" s="1"/>
+      <c r="D63" s="1"/>
+      <c r="E63" s="1"/>
+      <c r="F63" s="1"/>
+      <c r="G63" s="1"/>
+      <c r="H63" s="1"/>
+      <c r="I63" s="1"/>
+      <c r="J63" s="1"/>
+      <c r="K63" s="1"/>
+      <c r="L63" s="1"/>
+    </row>
+    <row r="64" spans="1:12">
+      <c r="A64" s="1"/>
+      <c r="B64" s="1"/>
+      <c r="C64" s="1"/>
+      <c r="D64" s="1"/>
+      <c r="E64" s="1"/>
+      <c r="F64" s="1"/>
+      <c r="G64" s="1"/>
+      <c r="H64" s="1"/>
+      <c r="I64" s="1"/>
+      <c r="J64" s="1"/>
+      <c r="K64" s="1"/>
+      <c r="L64" s="1"/>
     </row>
     <row r="65" spans="1:15">
-      <c r="A65" s="4"/>
-      <c r="B65" s="5"/>
-      <c r="C65" s="5"/>
-      <c r="D65" s="5"/>
-      <c r="E65" s="4"/>
-      <c r="F65" s="5"/>
-      <c r="G65" s="4">
-        <f t="shared" si="3"/>
-        <v>5440.3673807450004</v>
-      </c>
-      <c r="H65" s="1">
-        <v>-89823252.397523701</v>
-      </c>
-      <c r="I65" s="4"/>
-      <c r="J65" s="4"/>
-      <c r="K65" s="4"/>
-      <c r="L65" s="4">
-        <f t="shared" si="6"/>
-        <v>1.3298815693786121</v>
-      </c>
-      <c r="O65">
-        <v>4969.5380896440001</v>
-      </c>
+      <c r="A65" s="1"/>
+      <c r="B65" s="1"/>
+      <c r="C65" s="1"/>
+      <c r="D65" s="1"/>
+      <c r="E65" s="1"/>
+      <c r="F65" s="1"/>
+      <c r="G65" s="1"/>
+      <c r="H65" s="1"/>
+      <c r="I65" s="1"/>
+      <c r="J65" s="1"/>
+      <c r="K65" s="1"/>
+      <c r="L65" s="1"/>
     </row>
     <row r="66" spans="1:15">
-      <c r="A66" s="4"/>
-      <c r="B66" s="5"/>
-      <c r="C66" s="5"/>
-      <c r="D66" s="5"/>
-      <c r="E66" s="4"/>
-      <c r="F66" s="5"/>
-      <c r="G66" s="4"/>
-      <c r="H66" s="5"/>
-      <c r="I66" s="4"/>
-      <c r="J66" s="4"/>
-      <c r="K66" s="4"/>
-      <c r="L66" s="4"/>
+      <c r="A66" s="1"/>
+      <c r="B66" s="1"/>
+      <c r="C66" s="1"/>
+      <c r="D66" s="1"/>
+      <c r="E66" s="1"/>
+      <c r="F66" s="1"/>
+      <c r="G66" s="1"/>
+      <c r="H66" s="1"/>
+      <c r="I66" s="1"/>
+      <c r="J66" s="1"/>
+      <c r="K66" s="1"/>
+      <c r="L66" s="1"/>
       <c r="O66" s="1"/>
     </row>
     <row r="67" spans="1:15">
-      <c r="A67" s="4"/>
-      <c r="B67" s="5"/>
-      <c r="C67" s="4"/>
-      <c r="D67" s="4"/>
-      <c r="E67" s="4"/>
-      <c r="F67" s="5"/>
-      <c r="G67" s="4"/>
-      <c r="H67" s="5"/>
-      <c r="I67" s="4"/>
-      <c r="J67" s="4"/>
-      <c r="K67" s="4"/>
-      <c r="L67" s="4"/>
+      <c r="A67" s="1"/>
+      <c r="B67" s="1"/>
+      <c r="C67" s="1"/>
+      <c r="D67" s="1"/>
+      <c r="E67" s="1"/>
+      <c r="F67" s="1"/>
+      <c r="G67" s="1"/>
+      <c r="H67" s="1"/>
+      <c r="I67" s="1"/>
+      <c r="J67" s="1"/>
+      <c r="K67" s="1"/>
+      <c r="L67" s="1"/>
       <c r="O67" s="1"/>
     </row>
     <row r="68" spans="1:15">
-      <c r="A68" s="4"/>
-      <c r="B68" s="5"/>
-      <c r="C68" s="4"/>
-      <c r="D68" s="4"/>
-      <c r="E68" s="4"/>
-      <c r="F68" s="5"/>
-      <c r="G68" s="4"/>
-      <c r="H68" s="5"/>
-      <c r="I68" s="4"/>
-      <c r="J68" s="4"/>
-      <c r="K68" s="4"/>
-      <c r="L68" s="4"/>
+      <c r="A68" s="1"/>
+      <c r="B68" s="1"/>
+      <c r="C68" s="1"/>
+      <c r="D68" s="1"/>
+      <c r="E68" s="1"/>
+      <c r="F68" s="1"/>
+      <c r="G68" s="1"/>
+      <c r="H68" s="1"/>
+      <c r="I68" s="1"/>
+      <c r="J68" s="1"/>
+      <c r="K68" s="1"/>
+      <c r="L68" s="1"/>
       <c r="O68" s="1"/>
     </row>
     <row r="69" spans="1:15">
       <c r="B69" s="1"/>
       <c r="F69" s="1"/>
+      <c r="G69" s="1"/>
       <c r="H69" s="1"/>
+      <c r="I69" s="1"/>
+      <c r="J69" s="1"/>
+      <c r="K69" s="1"/>
+      <c r="L69" s="1"/>
     </row>
     <row r="70" spans="1:15">
       <c r="B70" s="1"/>

</xml_diff>